<commit_message>
Add inflation rate in expense assumption.
</commit_message>
<xml_diff>
--- a/export/LTPremTable.xlsx
+++ b/export/LTPremTable.xlsx
@@ -558,25 +558,25 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>1.19</v>
+        <v>1.16</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>0.71</v>
+        <v>0.68</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>1.78</v>
+        <v>1.76</v>
       </c>
       <c r="J3" t="s">
         <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>1.15</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="4">
@@ -584,25 +584,25 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>1.18</v>
+        <v>1.15</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="n">
-        <v>1.82</v>
+        <v>1.8</v>
       </c>
       <c r="J4" t="s">
         <v>4</v>
       </c>
       <c r="K4" t="n">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="5">
@@ -610,25 +610,25 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>1.18</v>
+        <v>1.15</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>0.76</v>
+        <v>0.73</v>
       </c>
       <c r="G5" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="n">
-        <v>1.86</v>
+        <v>1.84</v>
       </c>
       <c r="J5" t="s">
         <v>5</v>
       </c>
       <c r="K5" t="n">
-        <v>1.24</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="6">
@@ -636,25 +636,25 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>1.19</v>
+        <v>1.16</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.79</v>
+        <v>0.76</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="n">
-        <v>1.91</v>
+        <v>1.89</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
       </c>
       <c r="K6" t="n">
-        <v>1.29</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="7">
@@ -662,25 +662,25 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>1.2</v>
+        <v>1.17</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>0.83</v>
+        <v>0.8</v>
       </c>
       <c r="G7" t="s">
         <v>7</v>
       </c>
       <c r="H7" t="n">
-        <v>1.96</v>
+        <v>1.94</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
       </c>
       <c r="K7" t="n">
-        <v>1.34</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="8">
@@ -688,25 +688,25 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>0.88</v>
+        <v>0.85</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
       <c r="H8" t="n">
-        <v>2.03</v>
+        <v>2.01</v>
       </c>
       <c r="J8" t="s">
         <v>8</v>
       </c>
       <c r="K8" t="n">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="9">
@@ -714,25 +714,25 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>1.26</v>
+        <v>1.23</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>2.1</v>
+        <v>2.08</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
       </c>
       <c r="K9" t="n">
-        <v>1.47</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="10">
@@ -740,25 +740,25 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>1.3</v>
+        <v>1.27</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
       </c>
       <c r="H10" t="n">
-        <v>2.18</v>
+        <v>2.16</v>
       </c>
       <c r="J10" t="s">
         <v>10</v>
       </c>
       <c r="K10" t="n">
-        <v>1.53</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="11">
@@ -766,25 +766,25 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>1.35</v>
+        <v>1.32</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="n">
-        <v>1.04</v>
+        <v>1.01</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="n">
-        <v>2.27</v>
+        <v>2.25</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
       </c>
       <c r="K11" t="n">
-        <v>1.6</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="12">
@@ -792,25 +792,25 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>1.41</v>
+        <v>1.38</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>1.1</v>
+        <v>1.07</v>
       </c>
       <c r="G12" t="s">
         <v>12</v>
       </c>
       <c r="H12" t="n">
-        <v>2.36</v>
+        <v>2.34</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
       </c>
       <c r="K12" t="n">
-        <v>1.67</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="13">
@@ -818,25 +818,25 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>1.48</v>
+        <v>1.45</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="n">
-        <v>1.16</v>
+        <v>1.13</v>
       </c>
       <c r="G13" t="s">
         <v>13</v>
       </c>
       <c r="H13" t="n">
-        <v>2.46</v>
+        <v>2.43</v>
       </c>
       <c r="J13" t="s">
         <v>13</v>
       </c>
       <c r="K13" t="n">
-        <v>1.75</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="14">
@@ -844,25 +844,25 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>1.56</v>
+        <v>1.53</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>1.23</v>
+        <v>1.2</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>2.56</v>
+        <v>2.54</v>
       </c>
       <c r="J14" t="s">
         <v>14</v>
       </c>
       <c r="K14" t="n">
-        <v>1.83</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="15">
@@ -870,25 +870,25 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>1.65</v>
+        <v>1.62</v>
       </c>
       <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="n">
-        <v>1.31</v>
+        <v>1.28</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
       </c>
       <c r="H15" t="n">
-        <v>2.67</v>
+        <v>2.65</v>
       </c>
       <c r="J15" t="s">
         <v>15</v>
       </c>
       <c r="K15" t="n">
-        <v>1.91</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="16">
@@ -896,25 +896,25 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>1.75</v>
+        <v>1.72</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="n">
-        <v>1.4</v>
+        <v>1.37</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16" t="n">
-        <v>2.79</v>
+        <v>2.76</v>
       </c>
       <c r="J16" t="s">
         <v>16</v>
       </c>
       <c r="K16" t="n">
-        <v>2</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="17">
@@ -922,25 +922,25 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>1.87</v>
+        <v>1.84</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
       <c r="E17" t="n">
-        <v>1.49</v>
+        <v>1.46</v>
       </c>
       <c r="G17" t="s">
         <v>17</v>
       </c>
       <c r="H17" t="n">
-        <v>2.91</v>
+        <v>2.89</v>
       </c>
       <c r="J17" t="s">
         <v>17</v>
       </c>
       <c r="K17" t="n">
-        <v>2.09</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="18">
@@ -948,25 +948,25 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>1.97</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="E18" t="n">
-        <v>1.6</v>
+        <v>1.57</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
       <c r="H18" t="n">
-        <v>3.04</v>
+        <v>3.02</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
       </c>
       <c r="K18" t="n">
-        <v>2.18</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="19">
@@ -974,25 +974,25 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>2.16</v>
+        <v>2.13</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" t="n">
-        <v>1.71</v>
+        <v>1.68</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
       <c r="H19" t="n">
-        <v>3.18</v>
+        <v>3.16</v>
       </c>
       <c r="J19" t="s">
         <v>19</v>
       </c>
       <c r="K19" t="n">
-        <v>2.28</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="20">
@@ -1000,25 +1000,25 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>2.34</v>
+        <v>2.31</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
       <c r="E20" t="n">
-        <v>1.83</v>
+        <v>1.8</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
       </c>
       <c r="H20" t="n">
-        <v>3.34</v>
+        <v>3.31</v>
       </c>
       <c r="J20" t="s">
         <v>20</v>
       </c>
       <c r="K20" t="n">
-        <v>2.38</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="21">
@@ -1026,25 +1026,25 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>2.55</v>
+        <v>2.52</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="n">
-        <v>1.96</v>
+        <v>1.93</v>
       </c>
       <c r="G21" t="s">
         <v>21</v>
       </c>
       <c r="H21" t="n">
-        <v>3.5</v>
+        <v>3.47</v>
       </c>
       <c r="J21" t="s">
         <v>21</v>
       </c>
       <c r="K21" t="n">
-        <v>2.49</v>
+        <v>2.47</v>
       </c>
     </row>
     <row r="22">
@@ -1052,25 +1052,25 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>2.78</v>
+        <v>2.75</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="n">
-        <v>2.11</v>
+        <v>2.08</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
       </c>
       <c r="H22" t="n">
-        <v>3.67</v>
+        <v>3.64</v>
       </c>
       <c r="J22" t="s">
         <v>22</v>
       </c>
       <c r="K22" t="n">
-        <v>2.6</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="23">
@@ -1078,25 +1078,25 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>3.04</v>
+        <v>3.01</v>
       </c>
       <c r="D23" t="s">
         <v>23</v>
       </c>
       <c r="E23" t="n">
-        <v>2.26</v>
+        <v>2.23</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
       </c>
       <c r="H23" t="n">
-        <v>3.85</v>
+        <v>3.82</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
       <c r="K23" t="n">
-        <v>2.71</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="24">
@@ -1104,25 +1104,25 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>3.33</v>
+        <v>3.3</v>
       </c>
       <c r="D24" t="s">
         <v>24</v>
       </c>
       <c r="E24" t="n">
-        <v>2.43</v>
+        <v>2.4</v>
       </c>
       <c r="G24" t="s">
         <v>24</v>
       </c>
       <c r="H24" t="n">
-        <v>4.04</v>
+        <v>4.01</v>
       </c>
       <c r="J24" t="s">
         <v>24</v>
       </c>
       <c r="K24" t="n">
-        <v>2.82</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="25">
@@ -1130,25 +1130,25 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>3.65</v>
+        <v>3.62</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
       <c r="E25" t="n">
-        <v>2.62</v>
+        <v>2.58</v>
       </c>
       <c r="G25" t="s">
         <v>25</v>
       </c>
       <c r="H25" t="n">
-        <v>4.23</v>
+        <v>4.2</v>
       </c>
       <c r="J25" t="s">
         <v>25</v>
       </c>
       <c r="K25" t="n">
-        <v>2.94</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="26">
@@ -1156,25 +1156,25 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>4.01</v>
+        <v>3.98</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
       </c>
       <c r="E26" t="n">
-        <v>2.82</v>
+        <v>2.79</v>
       </c>
       <c r="G26" t="s">
         <v>26</v>
       </c>
       <c r="H26" t="n">
-        <v>4.43</v>
+        <v>4.4</v>
       </c>
       <c r="J26" t="s">
         <v>26</v>
       </c>
       <c r="K26" t="n">
-        <v>3.05</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="27">
@@ -1182,25 +1182,25 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>4.4</v>
+        <v>4.37</v>
       </c>
       <c r="D27" t="s">
         <v>27</v>
       </c>
       <c r="E27" t="n">
-        <v>3.04</v>
+        <v>3.01</v>
       </c>
       <c r="G27" t="s">
         <v>27</v>
       </c>
       <c r="H27" t="n">
-        <v>4.63</v>
+        <v>4.6</v>
       </c>
       <c r="J27" t="s">
         <v>27</v>
       </c>
       <c r="K27" t="n">
-        <v>3.17</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="28">
@@ -1208,25 +1208,25 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>4.83</v>
+        <v>4.8</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
       </c>
       <c r="E28" t="n">
-        <v>3.28</v>
+        <v>3.25</v>
       </c>
       <c r="G28" t="s">
         <v>28</v>
       </c>
       <c r="H28" t="n">
-        <v>4.83</v>
+        <v>4.8</v>
       </c>
       <c r="J28" t="s">
         <v>28</v>
       </c>
       <c r="K28" t="n">
-        <v>3.28</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="29">
@@ -1234,25 +1234,25 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>5.31</v>
+        <v>5.28</v>
       </c>
       <c r="D29" t="s">
         <v>29</v>
       </c>
       <c r="E29" t="n">
-        <v>3.55</v>
+        <v>3.52</v>
       </c>
       <c r="G29" t="s">
         <v>29</v>
       </c>
       <c r="H29" t="n">
-        <v>5.04</v>
+        <v>5</v>
       </c>
       <c r="J29" t="s">
         <v>29</v>
       </c>
       <c r="K29" t="n">
-        <v>3.4</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="30">
@@ -1260,25 +1260,25 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>5.83</v>
+        <v>5.8</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
       </c>
       <c r="E30" t="n">
-        <v>3.85</v>
+        <v>3.82</v>
       </c>
       <c r="G30" t="s">
         <v>30</v>
       </c>
       <c r="H30" t="n">
-        <v>5.23</v>
+        <v>5.2</v>
       </c>
       <c r="J30" t="s">
         <v>30</v>
       </c>
       <c r="K30" t="n">
-        <v>3.52</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="31">
@@ -1286,25 +1286,25 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>6.4</v>
+        <v>6.37</v>
       </c>
       <c r="D31" t="s">
         <v>31</v>
       </c>
       <c r="E31" t="n">
-        <v>4.18</v>
+        <v>4.15</v>
       </c>
       <c r="G31" t="s">
         <v>31</v>
       </c>
       <c r="H31" t="n">
-        <v>5.42</v>
+        <v>5.39</v>
       </c>
       <c r="J31" t="s">
         <v>31</v>
       </c>
       <c r="K31" t="n">
-        <v>3.63</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="32">
@@ -1312,25 +1312,25 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>7.03</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
       </c>
       <c r="E32" t="n">
-        <v>4.55</v>
+        <v>4.52</v>
       </c>
       <c r="G32" t="s">
         <v>32</v>
       </c>
       <c r="H32" t="n">
-        <v>5.6</v>
+        <v>5.56</v>
       </c>
       <c r="J32" t="s">
         <v>32</v>
       </c>
       <c r="K32" t="n">
-        <v>3.74</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="33">
@@ -1338,25 +1338,25 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>7.71</v>
+        <v>7.68</v>
       </c>
       <c r="D33" t="s">
         <v>33</v>
       </c>
       <c r="E33" t="n">
-        <v>4.95</v>
+        <v>4.92</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="H33" t="n">
-        <v>5.75</v>
+        <v>5.72</v>
       </c>
       <c r="J33" t="s">
         <v>33</v>
       </c>
       <c r="K33" t="n">
-        <v>3.84</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="34">
@@ -1364,25 +1364,25 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>8.46</v>
+        <v>8.43</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
       </c>
       <c r="E34" t="n">
-        <v>5.4</v>
+        <v>5.37</v>
       </c>
       <c r="G34" t="s">
         <v>34</v>
       </c>
       <c r="H34" t="n">
-        <v>5.9</v>
+        <v>5.87</v>
       </c>
       <c r="J34" t="s">
         <v>34</v>
       </c>
       <c r="K34" t="n">
-        <v>3.94</v>
+        <v>3.91</v>
       </c>
     </row>
     <row r="35">
@@ -1390,25 +1390,25 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>9.27</v>
+        <v>9.24</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
       </c>
       <c r="E35" t="n">
-        <v>5.9</v>
+        <v>5.87</v>
       </c>
       <c r="G35" t="s">
         <v>35</v>
       </c>
       <c r="H35" t="n">
-        <v>6.04</v>
+        <v>6.01</v>
       </c>
       <c r="J35" t="s">
         <v>35</v>
       </c>
       <c r="K35" t="n">
-        <v>4.04</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1416,25 +1416,25 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>10.15</v>
+        <v>10.12</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
       </c>
       <c r="E36" t="n">
-        <v>6.44</v>
+        <v>6.41</v>
       </c>
       <c r="G36" t="s">
         <v>36</v>
       </c>
       <c r="H36" t="n">
-        <v>6.18</v>
+        <v>6.14</v>
       </c>
       <c r="J36" t="s">
         <v>36</v>
       </c>
       <c r="K36" t="n">
-        <v>4.14</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="37">
@@ -1442,25 +1442,25 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>11.11</v>
+        <v>11.08</v>
       </c>
       <c r="D37" t="s">
         <v>37</v>
       </c>
       <c r="E37" t="n">
-        <v>7.05</v>
+        <v>7.02</v>
       </c>
       <c r="G37" t="s">
         <v>37</v>
       </c>
       <c r="H37" t="n">
-        <v>6.3</v>
+        <v>6.26</v>
       </c>
       <c r="J37" t="s">
         <v>37</v>
       </c>
       <c r="K37" t="n">
-        <v>4.23</v>
+        <v>4.19</v>
       </c>
     </row>
     <row r="38">
@@ -1468,25 +1468,25 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>12.15</v>
+        <v>12.12</v>
       </c>
       <c r="D38" t="s">
         <v>38</v>
       </c>
       <c r="E38" t="n">
-        <v>7.71</v>
+        <v>7.68</v>
       </c>
       <c r="G38" t="s">
         <v>38</v>
       </c>
       <c r="H38" t="n">
-        <v>6.41</v>
+        <v>6.37</v>
       </c>
       <c r="J38" t="s">
         <v>38</v>
       </c>
       <c r="K38" t="n">
-        <v>4.33</v>
+        <v>4.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>